<commit_message>
fixed to use the filtered df to calcualtae cate
</commit_message>
<xml_diff>
--- a/algorithms/algorithm_time.xlsx
+++ b/algorithms/algorithm_time.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1788,21 +1788,735 @@
           <t>{'RaceEthnicity': 'White or of European descent'}</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>20000</t>
-        </is>
+      <c r="E40" t="n">
+        <v>21</v>
+      </c>
+      <c r="F40" t="n">
+        <v>20000</v>
       </c>
       <c r="G40" t="n">
         <v>8.241000874000747</v>
       </c>
       <c r="H40" t="n">
         <v>0.1373500145666791</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2025-06-25 17:52:11</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>NaiveDFS</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>{'Exercise': '3 - 4 times per week'}</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>{'RaceEthnicity': 'White or of European descent'}</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>4</v>
+      </c>
+      <c r="F41" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G41" t="n">
+        <v>20.26472453499809</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0.3377454089166349</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2025-06-25 17:52:12</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Apriori</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>{'Exercise': '3 - 4 times per week'}</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>{'RaceEthnicity': 'White or of European descent'}</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0.6112939700033166</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0.01018823283338861</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2025-06-25 17:52:18</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>FP</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>{'Exercise': '3 - 4 times per week'}</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>{'RaceEthnicity': 'White or of European descent'}</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G43" t="n">
+        <v>5.423727711000538</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0.09039546185000896</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2025-06-25 20:08:03</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>NaiveDFS</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>{'Exercise': '3 - 4 times per week'}</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>{'RaceEthnicity': 'White or of European descent'}</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>25</v>
+      </c>
+      <c r="F44" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G44" t="n">
+        <v>18.42766634200234</v>
+      </c>
+      <c r="H44" t="n">
+        <v>0.3071277723667057</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2025-06-25 20:08:34</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>NaiveDFS</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>{'HoursComputer': '5 - 8 hours'}</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>{'Gender': 'Male'}</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>33</v>
+      </c>
+      <c r="F45" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G45" t="n">
+        <v>30.30420459100424</v>
+      </c>
+      <c r="H45" t="n">
+        <v>0.5050700765167373</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2025-06-25 20:09:14</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>NaiveDFS</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>{'HoursComputer': '1 - 4 hours', 'FormalEducation': 'Master’s degree (MA, MS, M.Eng., MBA, etc.)'}</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>{'RaceEthnicity': 'White or of European descent'}</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>43</v>
+      </c>
+      <c r="F46" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G46" t="n">
+        <v>40.33883208200132</v>
+      </c>
+      <c r="H46" t="n">
+        <v>0.6723138680333552</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2025-06-25 20:23:09</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>NaiveDFS</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>{'Exercise': '3 - 4 times per week'}</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>{'RaceEthnicity': 'White or of European descent'}</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>21</v>
+      </c>
+      <c r="F47" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G47" t="n">
+        <v>27.50110511200182</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0.4583517518666971</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2025-06-25 20:24:15</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>NaiveDFS</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>{'HoursComputer': '5 - 8 hours'}</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>{'Gender': 'Male'}</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>29</v>
+      </c>
+      <c r="F48" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G48" t="n">
+        <v>64.83382585099753</v>
+      </c>
+      <c r="H48" t="n">
+        <v>1.080563764183292</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2025-06-25 20:25:06</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>NaiveDFS</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>{'HoursComputer': '1 - 4 hours', 'FormalEducation': 'Master’s degree (MA, MS, M.Eng., MBA, etc.)'}</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>{'RaceEthnicity': 'White or of European descent'}</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v>21</v>
+      </c>
+      <c r="F49" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G49" t="n">
+        <v>49.95099182800186</v>
+      </c>
+      <c r="H49" t="n">
+        <v>0.8325165304666977</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2025-06-25 21:21:48</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Apriori</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>{'Exercise': '3 - 4 times per week'}</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>{'RaceEthnicity': 'White or of European descent'}</t>
+        </is>
+      </c>
+      <c r="E50" t="n">
+        <v>0</v>
+      </c>
+      <c r="F50" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G50" t="n">
+        <v>0.5756943699961994</v>
+      </c>
+      <c r="H50" t="n">
+        <v>0.009594906166603323</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2025-06-25 21:21:48</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Apriori</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>{'HoursComputer': '5 - 8 hours'}</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>{'Gender': 'Male'}</t>
+        </is>
+      </c>
+      <c r="E51" t="n">
+        <v>0</v>
+      </c>
+      <c r="F51" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G51" t="n">
+        <v>0.6204752510020626</v>
+      </c>
+      <c r="H51" t="n">
+        <v>0.01034125418336771</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2025-06-25 21:21:50</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Apriori</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>{'HoursComputer': '1 - 4 hours', 'FormalEducation': 'Master’s degree (MA, MS, M.Eng., MBA, etc.)'}</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>{'RaceEthnicity': 'White or of European descent'}</t>
+        </is>
+      </c>
+      <c r="E52" t="n">
+        <v>0</v>
+      </c>
+      <c r="F52" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G52" t="n">
+        <v>0.6244888240034925</v>
+      </c>
+      <c r="H52" t="n">
+        <v>0.01040814706672488</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2025-06-25 21:36:23</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Apriori</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>{'Exercise': '3 - 4 times per week'}</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>{'RaceEthnicity': 'White or of European descent'}</t>
+        </is>
+      </c>
+      <c r="E53" t="n">
+        <v>25</v>
+      </c>
+      <c r="F53" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G53" t="n">
+        <v>0.9656246330050635</v>
+      </c>
+      <c r="H53" t="n">
+        <v>0.01609374388341773</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2025-06-25 21:36:25</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Apriori</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>{'HoursComputer': '5 - 8 hours'}</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>{'Gender': 'Male'}</t>
+        </is>
+      </c>
+      <c r="E54" t="n">
+        <v>33</v>
+      </c>
+      <c r="F54" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G54" t="n">
+        <v>1.457824452998466</v>
+      </c>
+      <c r="H54" t="n">
+        <v>0.0242970742166411</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2025-06-25 21:36:27</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Apriori</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>{'HoursComputer': '1 - 4 hours', 'FormalEducation': 'Master’s degree (MA, MS, M.Eng., MBA, etc.)'}</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>{'RaceEthnicity': 'White or of European descent'}</t>
+        </is>
+      </c>
+      <c r="E55" t="n">
+        <v>43</v>
+      </c>
+      <c r="F55" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G55" t="n">
+        <v>1.569658543005062</v>
+      </c>
+      <c r="H55" t="n">
+        <v>0.02616097571675103</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2025-06-25 21:39:58</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Apriori</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>{'Exercise': '3 - 4 times per week'}</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>{'RaceEthnicity': 'White or of European descent'}</t>
+        </is>
+      </c>
+      <c r="E56" t="n">
+        <v>21</v>
+      </c>
+      <c r="F56" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G56" t="n">
+        <v>2.618635594000807</v>
+      </c>
+      <c r="H56" t="n">
+        <v>0.04364392656668012</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2025-06-25 21:40:01</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Apriori</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>{'HoursComputer': '5 - 8 hours'}</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>{'Gender': 'Male'}</t>
+        </is>
+      </c>
+      <c r="E57" t="n">
+        <v>29</v>
+      </c>
+      <c r="F57" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G57" t="n">
+        <v>2.74235752900131</v>
+      </c>
+      <c r="H57" t="n">
+        <v>0.04570595881668851</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2025-06-25 21:40:04</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Apriori</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>{'HoursComputer': '1 - 4 hours', 'FormalEducation': 'Master’s degree (MA, MS, M.Eng., MBA, etc.)'}</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>{'RaceEthnicity': 'White or of European descent'}</t>
+        </is>
+      </c>
+      <c r="E58" t="n">
+        <v>21</v>
+      </c>
+      <c r="F58" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G58" t="n">
+        <v>1.559883781999815</v>
+      </c>
+      <c r="H58" t="n">
+        <v>0.02599806303333025</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2025-06-25 21:54:16</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>FP</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>{'Exercise': '3 - 4 times per week'}</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>{'RaceEthnicity': 'White or of European descent'}</t>
+        </is>
+      </c>
+      <c r="E59" t="n">
+        <v>21</v>
+      </c>
+      <c r="F59" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G59" t="n">
+        <v>0.8526472130033653</v>
+      </c>
+      <c r="H59" t="n">
+        <v>0.01421078688338942</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2025-06-25 21:54:18</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>FP</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>{'HoursComputer': '5 - 8 hours'}</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>{'Gender': 'Male'}</t>
+        </is>
+      </c>
+      <c r="E60" t="n">
+        <v>29</v>
+      </c>
+      <c r="F60" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G60" t="n">
+        <v>1.825525783002377</v>
+      </c>
+      <c r="H60" t="n">
+        <v>0.03042542971670627</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2025-06-25 21:54:20</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>FP</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>{'HoursComputer': '1 - 4 hours', 'FormalEducation': 'Master’s degree (MA, MS, M.Eng., MBA, etc.)'}</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>{'RaceEthnicity': 'White or of European descent'}</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>20000</t>
+        </is>
+      </c>
+      <c r="G61" t="n">
+        <v>1.416913036999176</v>
+      </c>
+      <c r="H61" t="n">
+        <v>0.0236152172833196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>